<commit_message>
Nova vers~so do chromedriver
Commit para atualizar a versão do chromedriver para a 97
</commit_message>
<xml_diff>
--- a/automacaoWebEBuscaDeInformacoes/Produtos Atualizados.xlsx
+++ b/automacaoWebEBuscaDeInformacoes/Produtos Atualizados.xlsx
@@ -67,55 +67,55 @@
     <t>Ouro</t>
   </si>
   <si>
-    <t>5.34</t>
-  </si>
-  <si>
-    <t>6.47</t>
-  </si>
-  <si>
-    <t>304.29</t>
-  </si>
-  <si>
-    <t>5337.95</t>
-  </si>
-  <si>
-    <t>29121.86</t>
-  </si>
-  <si>
-    <t>4804.15</t>
-  </si>
-  <si>
-    <t>4265.06</t>
-  </si>
-  <si>
-    <t>19414.57</t>
-  </si>
-  <si>
-    <t>2564.80</t>
-  </si>
-  <si>
-    <t>6085.80</t>
-  </si>
-  <si>
-    <t>7473.13</t>
-  </si>
-  <si>
-    <t>58243.72</t>
-  </si>
-  <si>
-    <t>8167.05</t>
-  </si>
-  <si>
-    <t>7250.61</t>
-  </si>
-  <si>
-    <t>36887.69</t>
-  </si>
-  <si>
-    <t>5129.60</t>
-  </si>
-  <si>
-    <t>6998.67</t>
+    <t>5.64</t>
+  </si>
+  <si>
+    <t>6.40</t>
+  </si>
+  <si>
+    <t>325.48</t>
+  </si>
+  <si>
+    <t>5635.74</t>
+  </si>
+  <si>
+    <t>28812.75</t>
+  </si>
+  <si>
+    <t>5072.16</t>
+  </si>
+  <si>
+    <t>4503.00</t>
+  </si>
+  <si>
+    <t>19208.50</t>
+  </si>
+  <si>
+    <t>2707.89</t>
+  </si>
+  <si>
+    <t>6509.60</t>
+  </si>
+  <si>
+    <t>7890.04</t>
+  </si>
+  <si>
+    <t>57625.49</t>
+  </si>
+  <si>
+    <t>8622.68</t>
+  </si>
+  <si>
+    <t>7655.11</t>
+  </si>
+  <si>
+    <t>36496.14</t>
+  </si>
+  <si>
+    <t>5415.78</t>
+  </si>
+  <si>
+    <t>7486.04</t>
   </si>
 </sst>
 </file>

</xml_diff>